<commit_message>
updated trend analysis functions to perform primary, time series, and secondary analysis from the hazard interpretation template.These functions still need testing. Explored clustering topic modeling results.
</commit_message>
<xml_diff>
--- a/output data/hazard_interpretation_template.xlsx
+++ b/output data/hazard_interpretation_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A323364-2065-40BF-88D2-434C6AB2698F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328E1235-8B99-42EA-A496-1C1A4406A7C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="10044" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Hazard words</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Relevant Category words</t>
+  </si>
+  <si>
+    <t>Negation words</t>
   </si>
 </sst>
 </file>
@@ -431,36 +434,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD202B9-4913-4B48-97F7-AC087D3F80D8}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -474,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cleaned up and removed old data
</commit_message>
<xml_diff>
--- a/output data/hazard_interpretation_template.xlsx
+++ b/output data/hazard_interpretation_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328E1235-8B99-42EA-A496-1C1A4406A7C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2250C6F8-1263-40D0-B938-B79B21C90979}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="10044" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="1764" yWindow="2820" windowWidth="13824" windowHeight="8040" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Hazard words</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -74,6 +71,12 @@
   </si>
   <si>
     <t>Negation words</t>
+  </si>
+  <si>
+    <t>Action/Descriptor</t>
+  </si>
+  <si>
+    <t>Hazard Noun/Subject</t>
   </si>
 </sst>
 </file>
@@ -437,37 +440,43 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -488,29 +497,29 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated topic-focused template to match functions
</commit_message>
<xml_diff>
--- a/output data/hazard_interpretation_template.xlsx
+++ b/output data/hazard_interpretation_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2250C6F8-1263-40D0-B938-B79B21C90979}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAADCAC9-E862-454B-B09A-3E998EE8A41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1764" yWindow="2820" windowWidth="13824" windowHeight="8040" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="-19410" yWindow="-450" windowWidth="17280" windowHeight="10050" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD202B9-4913-4B48-97F7-AC087D3F80D8}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,15 +487,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -520,6 +520,16 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>